<commit_message>
Se agregan nuevos objetos en el login
Se agregaron dos objetos en el login porque se actualizo la pagina de inicio
</commit_message>
<xml_diff>
--- a/Components/Siniestros/Default.xlsx
+++ b/Components/Siniestros/Default.xlsx
@@ -302,10 +302,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
@@ -611,14 +611,14 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="18" width="9.41796875" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="9.078125" style="5" customWidth="1"/>
+    <col min="1" max="18" width="9.41796875" style="4" customWidth="1"/>
+    <col min="19" max="16384" width="9.078125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" s="8" customFormat="1">
@@ -682,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>1000354</v>
+        <v>1000358</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -690,7 +690,7 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -705,7 +705,7 @@
       <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="2">
@@ -748,7 +748,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="5" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>

<commit_message>
se ajusta componentes de siniestros al momento de cerrar el navegador
</commit_message>
<xml_diff>
--- a/Components/Siniestros/Default.xlsx
+++ b/Components/Siniestros/Default.xlsx
@@ -302,17 +302,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,16 +612,16 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="18" width="9.41796875" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="9.078125" style="4" customWidth="1"/>
+    <col min="1" max="18" width="9.41796875" style="5" customWidth="1"/>
+    <col min="19" max="16384" width="9.078125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="8" customFormat="1">
+    <row r="1" ht="14.95" s="7" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -673,7 +673,7 @@
       <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -690,7 +690,7 @@
       <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -705,7 +705,7 @@
       <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="2">
@@ -748,7 +748,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="4" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>

</xml_diff>